<commit_message>
mentor-dashboard/fix - fix problem with rows
</commit_message>
<xml_diff>
--- a/mentor-dashboard/src/data/Tasks.xlsx
+++ b/mentor-dashboard/src/data/Tasks.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RSSCHOOL\saniok017-2018Q3\mentor-dashboard\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +97,7 @@
     <t>Course work</t>
   </si>
   <si>
-    <t>RS Activist</t>
+    <t>RS Activist -</t>
   </si>
 </sst>
 </file>
@@ -435,7 +430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,10 +447,10 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="89.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="89.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">

</xml_diff>